<commit_message>
Regenerated outputs for SML where multiple changes have been done such as - invariants and their descriptions - changes in terminology bindings - Cardinality changes
etc.

CIFMM-2712
</commit_message>
<xml_diff>
--- a/output/SharedMedicinesList/list-sml-pracchanges-1.xlsx
+++ b/output/SharedMedicinesList/list-sml-pracchanges-1.xlsx
@@ -640,7 +640,7 @@
     <t>Lists often contain subsets of resources rather than an exhaustive list.  The code identifies what type of subset is included.</t>
   </si>
   <si>
-    <t>https://healthterminologies.gov.au/fhir/ValueSet/medicines-list-type-1</t>
+    <t>https://healthterminologies.gov.au/fhir/ValueSet/history-of-medication-use-type-1</t>
   </si>
   <si>
     <t>.code</t>
@@ -1209,7 +1209,7 @@
     <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="95.21875" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="73.671875" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="75.7109375" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="40.03515625" customWidth="true" bestFit="true"/>

</xml_diff>

<commit_message>
SML FHIR IG with extension Dose Administration Aid Medicines Indicator referenced by the List profile
</commit_message>
<xml_diff>
--- a/output/SharedMedicinesList/list-sml-pracchanges-1.xlsx
+++ b/output/SharedMedicinesList/list-sml-pracchanges-1.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AK$50</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AK$51</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1648" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1681" uniqueCount="326">
   <si>
     <t>Path</t>
   </si>
@@ -506,6 +506,19 @@
   </si>
   <si>
     <t>The entity (related person) responsible for deciding what the contents of the list were. Where the list was created by a human, this is the same as the author of the list.</t>
+  </si>
+  <si>
+    <t>packed-in-daa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/packed-in-daa-1}
+</t>
+  </si>
+  <si>
+    <t>Inclusion of medicines packed in a Dose Administration Aid (DAA) indicator</t>
+  </si>
+  <si>
+    <t>Indicates whether one or more items in a medicines list are packed in a Dose Administration Aid (DAA).</t>
   </si>
   <si>
     <t>List.modifierExtension</t>
@@ -1172,7 +1185,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AK50"/>
+  <dimension ref="A1:AK51"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1191,7 +1204,7 @@
     <col min="8" max="8" width="11.98828125" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="12.74609375" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="59.1953125" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="67.921875" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -3108,13 +3121,15 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" hidden="true">
+    <row r="19">
       <c r="A19" t="s" s="2">
+        <v>142</v>
+      </c>
+      <c r="B19" t="s" s="2">
         <v>156</v>
       </c>
-      <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
-        <v>68</v>
+        <v>41</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" t="s" s="2">
@@ -3124,26 +3139,24 @@
         <v>40</v>
       </c>
       <c r="G19" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="H19" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="I19" t="s" s="2">
         <v>41</v>
       </c>
       <c r="J19" t="s" s="2">
-        <v>69</v>
+        <v>157</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>158</v>
-      </c>
-      <c r="M19" t="s" s="2">
-        <v>72</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="M19" s="2"/>
       <c r="N19" s="2"/>
       <c r="O19" t="s" s="2">
         <v>41</v>
@@ -3192,7 +3205,7 @@
         <v>41</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>39</v>
@@ -3207,7 +3220,7 @@
         <v>41</v>
       </c>
       <c r="AJ19" t="s" s="2">
-        <v>141</v>
+        <v>41</v>
       </c>
       <c r="AK19" t="s" s="2">
         <v>41</v>
@@ -3219,7 +3232,7 @@
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
-        <v>41</v>
+        <v>68</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" t="s" s="2">
@@ -3232,21 +3245,23 @@
         <v>41</v>
       </c>
       <c r="H20" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="I20" t="s" s="2">
         <v>41</v>
       </c>
       <c r="J20" t="s" s="2">
+        <v>69</v>
+      </c>
+      <c r="K20" t="s" s="2">
         <v>161</v>
       </c>
-      <c r="K20" t="s" s="2">
+      <c r="L20" t="s" s="2">
         <v>162</v>
       </c>
-      <c r="L20" t="s" s="2">
-        <v>163</v>
-      </c>
-      <c r="M20" s="2"/>
+      <c r="M20" t="s" s="2">
+        <v>72</v>
+      </c>
       <c r="N20" s="2"/>
       <c r="O20" t="s" s="2">
         <v>41</v>
@@ -3295,7 +3310,7 @@
         <v>41</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>39</v>
@@ -3310,15 +3325,15 @@
         <v>41</v>
       </c>
       <c r="AJ20" t="s" s="2">
+        <v>141</v>
+      </c>
+      <c r="AK20" t="s" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" hidden="true">
+      <c r="A21" t="s" s="2">
         <v>164</v>
-      </c>
-      <c r="AK20" t="s" s="2">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s" s="2">
-        <v>166</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
@@ -3326,104 +3341,102 @@
       </c>
       <c r="D21" s="2"/>
       <c r="E21" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="F21" t="s" s="2">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="G21" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="H21" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="I21" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>117</v>
+        <v>165</v>
       </c>
       <c r="K21" t="s" s="2">
+        <v>166</v>
+      </c>
+      <c r="L21" t="s" s="2">
         <v>167</v>
       </c>
-      <c r="L21" t="s" s="2">
-        <v>168</v>
-      </c>
-      <c r="M21" t="s" s="2">
-        <v>169</v>
-      </c>
+      <c r="M21" s="2"/>
       <c r="N21" s="2"/>
       <c r="O21" t="s" s="2">
         <v>41</v>
       </c>
       <c r="P21" s="2"/>
       <c r="Q21" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="R21" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="S21" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="T21" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="U21" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="V21" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="W21" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="X21" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Y21" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Z21" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA21" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AB21" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AC21" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD21" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AE21" t="s" s="2">
+        <v>164</v>
+      </c>
+      <c r="AF21" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG21" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AH21" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AI21" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AJ21" t="s" s="2">
+        <v>168</v>
+      </c>
+      <c r="AK21" t="s" s="2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="2">
         <v>170</v>
-      </c>
-      <c r="R21" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S21" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T21" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U21" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V21" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W21" t="s" s="2">
-        <v>171</v>
-      </c>
-      <c r="X21" t="s" s="2">
-        <v>172</v>
-      </c>
-      <c r="Y21" t="s" s="2">
-        <v>173</v>
-      </c>
-      <c r="Z21" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA21" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB21" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC21" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD21" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE21" t="s" s="2">
-        <v>166</v>
-      </c>
-      <c r="AF21" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="AG21" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="AH21" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI21" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ21" t="s" s="2">
-        <v>174</v>
-      </c>
-      <c r="AK21" t="s" s="2">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="22" hidden="true">
-      <c r="A22" t="s" s="2">
-        <v>176</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
@@ -3437,7 +3450,7 @@
         <v>48</v>
       </c>
       <c r="G22" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="H22" t="s" s="2">
         <v>49</v>
@@ -3449,23 +3462,21 @@
         <v>117</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>179</v>
-      </c>
-      <c r="N22" t="s" s="2">
-        <v>180</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="N22" s="2"/>
       <c r="O22" t="s" s="2">
         <v>41</v>
       </c>
       <c r="P22" s="2"/>
       <c r="Q22" t="s" s="2">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="R22" t="s" s="2">
         <v>41</v>
@@ -3483,13 +3494,13 @@
         <v>41</v>
       </c>
       <c r="W22" t="s" s="2">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="X22" t="s" s="2">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="Y22" t="s" s="2">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="Z22" t="s" s="2">
         <v>41</v>
@@ -3507,7 +3518,7 @@
         <v>41</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>48</v>
@@ -3522,15 +3533,15 @@
         <v>41</v>
       </c>
       <c r="AJ22" t="s" s="2">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="AK22" t="s" s="2">
-        <v>185</v>
+        <v>179</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -3538,45 +3549,47 @@
       </c>
       <c r="D23" s="2"/>
       <c r="E23" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="F23" t="s" s="2">
         <v>48</v>
       </c>
       <c r="G23" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H23" t="s" s="2">
         <v>49</v>
-      </c>
-      <c r="H23" t="s" s="2">
-        <v>41</v>
       </c>
       <c r="I23" t="s" s="2">
         <v>49</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>62</v>
+        <v>117</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>188</v>
-      </c>
-      <c r="M23" s="2"/>
+        <v>182</v>
+      </c>
+      <c r="M23" t="s" s="2">
+        <v>183</v>
+      </c>
       <c r="N23" t="s" s="2">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="O23" t="s" s="2">
         <v>41</v>
       </c>
       <c r="P23" s="2"/>
       <c r="Q23" t="s" s="2">
-        <v>41</v>
+        <v>185</v>
       </c>
       <c r="R23" t="s" s="2">
         <v>41</v>
       </c>
       <c r="S23" t="s" s="2">
-        <v>190</v>
+        <v>41</v>
       </c>
       <c r="T23" t="s" s="2">
         <v>41</v>
@@ -3588,13 +3601,13 @@
         <v>41</v>
       </c>
       <c r="W23" t="s" s="2">
-        <v>41</v>
+        <v>175</v>
       </c>
       <c r="X23" t="s" s="2">
-        <v>41</v>
+        <v>186</v>
       </c>
       <c r="Y23" t="s" s="2">
-        <v>41</v>
+        <v>187</v>
       </c>
       <c r="Z23" t="s" s="2">
         <v>41</v>
@@ -3612,10 +3625,10 @@
         <v>41</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="AF23" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="AG23" t="s" s="2">
         <v>48</v>
@@ -3627,15 +3640,15 @@
         <v>41</v>
       </c>
       <c r="AJ23" t="s" s="2">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>41</v>
+        <v>189</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="2">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -3643,7 +3656,7 @@
       </c>
       <c r="D24" s="2"/>
       <c r="E24" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="F24" t="s" s="2">
         <v>48</v>
@@ -3658,19 +3671,17 @@
         <v>49</v>
       </c>
       <c r="J24" t="s" s="2">
+        <v>62</v>
+      </c>
+      <c r="K24" t="s" s="2">
+        <v>191</v>
+      </c>
+      <c r="L24" t="s" s="2">
+        <v>192</v>
+      </c>
+      <c r="M24" s="2"/>
+      <c r="N24" t="s" s="2">
         <v>193</v>
-      </c>
-      <c r="K24" t="s" s="2">
-        <v>194</v>
-      </c>
-      <c r="L24" t="s" s="2">
-        <v>195</v>
-      </c>
-      <c r="M24" t="s" s="2">
-        <v>196</v>
-      </c>
-      <c r="N24" t="s" s="2">
-        <v>197</v>
       </c>
       <c r="O24" t="s" s="2">
         <v>41</v>
@@ -3683,7 +3694,7 @@
         <v>41</v>
       </c>
       <c r="S24" t="s" s="2">
-        <v>41</v>
+        <v>194</v>
       </c>
       <c r="T24" t="s" s="2">
         <v>41</v>
@@ -3695,11 +3706,13 @@
         <v>41</v>
       </c>
       <c r="W24" t="s" s="2">
-        <v>171</v>
-      </c>
-      <c r="X24" s="2"/>
+        <v>41</v>
+      </c>
+      <c r="X24" t="s" s="2">
+        <v>41</v>
+      </c>
       <c r="Y24" t="s" s="2">
-        <v>198</v>
+        <v>41</v>
       </c>
       <c r="Z24" t="s" s="2">
         <v>41</v>
@@ -3717,7 +3730,7 @@
         <v>41</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>39</v>
@@ -3732,15 +3745,15 @@
         <v>41</v>
       </c>
       <c r="AJ24" t="s" s="2">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="AK24" t="s" s="2">
-        <v>200</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="2">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -3763,19 +3776,19 @@
         <v>49</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="N25" t="s" s="2">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="O25" t="s" s="2">
         <v>41</v>
@@ -3800,13 +3813,11 @@
         <v>41</v>
       </c>
       <c r="W25" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="X25" t="s" s="2">
-        <v>41</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="X25" s="2"/>
       <c r="Y25" t="s" s="2">
-        <v>41</v>
+        <v>202</v>
       </c>
       <c r="Z25" t="s" s="2">
         <v>41</v>
@@ -3824,7 +3835,7 @@
         <v>41</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>39</v>
@@ -3839,15 +3850,15 @@
         <v>41</v>
       </c>
       <c r="AJ25" t="s" s="2">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="2">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -3855,7 +3866,7 @@
       </c>
       <c r="D26" s="2"/>
       <c r="E26" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="F26" t="s" s="2">
         <v>48</v>
@@ -3867,19 +3878,23 @@
         <v>41</v>
       </c>
       <c r="I26" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="J26" t="s" s="2">
+        <v>206</v>
+      </c>
+      <c r="K26" t="s" s="2">
+        <v>207</v>
+      </c>
+      <c r="L26" t="s" s="2">
+        <v>208</v>
+      </c>
+      <c r="M26" t="s" s="2">
+        <v>209</v>
+      </c>
+      <c r="N26" t="s" s="2">
         <v>210</v>
       </c>
-      <c r="K26" t="s" s="2">
-        <v>211</v>
-      </c>
-      <c r="L26" t="s" s="2">
-        <v>212</v>
-      </c>
-      <c r="M26" s="2"/>
-      <c r="N26" s="2"/>
       <c r="O26" t="s" s="2">
         <v>41</v>
       </c>
@@ -3927,7 +3942,7 @@
         <v>41</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>39</v>
@@ -3942,15 +3957,15 @@
         <v>41</v>
       </c>
       <c r="AJ26" t="s" s="2">
+        <v>211</v>
+      </c>
+      <c r="AK26" t="s" s="2">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="2">
         <v>213</v>
-      </c>
-      <c r="AK26" t="s" s="2">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="27" hidden="true">
-      <c r="A27" t="s" s="2">
-        <v>215</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -3964,7 +3979,7 @@
         <v>48</v>
       </c>
       <c r="G27" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="H27" t="s" s="2">
         <v>41</v>
@@ -3973,13 +3988,13 @@
         <v>41</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>62</v>
+        <v>214</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>63</v>
+        <v>215</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>64</v>
+        <v>216</v>
       </c>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
@@ -4030,7 +4045,7 @@
         <v>41</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>65</v>
+        <v>213</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>39</v>
@@ -4045,26 +4060,26 @@
         <v>41</v>
       </c>
       <c r="AJ27" t="s" s="2">
-        <v>66</v>
+        <v>217</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>41</v>
+        <v>218</v>
       </c>
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
-        <v>68</v>
+        <v>41</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" t="s" s="2">
         <v>39</v>
       </c>
       <c r="F28" t="s" s="2">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="G28" t="s" s="2">
         <v>41</v>
@@ -4076,17 +4091,15 @@
         <v>41</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="M28" t="s" s="2">
-        <v>72</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="M28" s="2"/>
       <c r="N28" s="2"/>
       <c r="O28" t="s" s="2">
         <v>41</v>
@@ -4123,25 +4136,25 @@
         <v>41</v>
       </c>
       <c r="AA28" t="s" s="2">
-        <v>73</v>
+        <v>41</v>
       </c>
       <c r="AB28" t="s" s="2">
-        <v>74</v>
+        <v>41</v>
       </c>
       <c r="AC28" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AD28" t="s" s="2">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG28" t="s" s="2">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="AH28" t="s" s="2">
         <v>41</v>
@@ -4158,18 +4171,18 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
-        <v>41</v>
+        <v>68</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="F29" t="s" s="2">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="G29" t="s" s="2">
         <v>41</v>
@@ -4178,19 +4191,19 @@
         <v>41</v>
       </c>
       <c r="I29" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>218</v>
+        <v>70</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>219</v>
+        <v>71</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>220</v>
+        <v>72</v>
       </c>
       <c r="N29" s="2"/>
       <c r="O29" t="s" s="2">
@@ -4228,34 +4241,34 @@
         <v>41</v>
       </c>
       <c r="AA29" t="s" s="2">
-        <v>41</v>
+        <v>73</v>
       </c>
       <c r="AB29" t="s" s="2">
-        <v>41</v>
+        <v>74</v>
       </c>
       <c r="AC29" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AD29" t="s" s="2">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>221</v>
+        <v>76</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG29" t="s" s="2">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="AH29" t="s" s="2">
-        <v>222</v>
+        <v>41</v>
       </c>
       <c r="AI29" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AJ29" t="s" s="2">
-        <v>141</v>
+        <v>66</v>
       </c>
       <c r="AK29" t="s" s="2">
         <v>41</v>
@@ -4263,7 +4276,7 @@
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4271,7 +4284,7 @@
       </c>
       <c r="D30" s="2"/>
       <c r="E30" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="F30" t="s" s="2">
         <v>48</v>
@@ -4286,16 +4299,16 @@
         <v>49</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>161</v>
+        <v>62</v>
       </c>
       <c r="K30" t="s" s="2">
+        <v>222</v>
+      </c>
+      <c r="L30" t="s" s="2">
+        <v>223</v>
+      </c>
+      <c r="M30" t="s" s="2">
         <v>224</v>
-      </c>
-      <c r="L30" t="s" s="2">
-        <v>225</v>
-      </c>
-      <c r="M30" t="s" s="2">
-        <v>226</v>
       </c>
       <c r="N30" s="2"/>
       <c r="O30" t="s" s="2">
@@ -4345,7 +4358,7 @@
         <v>41</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>39</v>
@@ -4354,13 +4367,13 @@
         <v>48</v>
       </c>
       <c r="AH30" t="s" s="2">
-        <v>41</v>
+        <v>226</v>
       </c>
       <c r="AI30" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AJ30" t="s" s="2">
-        <v>228</v>
+        <v>141</v>
       </c>
       <c r="AK30" t="s" s="2">
         <v>41</v>
@@ -4368,7 +4381,7 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -4391,16 +4404,16 @@
         <v>49</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>62</v>
+        <v>165</v>
       </c>
       <c r="K31" t="s" s="2">
+        <v>228</v>
+      </c>
+      <c r="L31" t="s" s="2">
+        <v>229</v>
+      </c>
+      <c r="M31" t="s" s="2">
         <v>230</v>
-      </c>
-      <c r="L31" t="s" s="2">
-        <v>231</v>
-      </c>
-      <c r="M31" t="s" s="2">
-        <v>232</v>
       </c>
       <c r="N31" s="2"/>
       <c r="O31" t="s" s="2">
@@ -4450,30 +4463,30 @@
         <v>41</v>
       </c>
       <c r="AE31" t="s" s="2">
+        <v>231</v>
+      </c>
+      <c r="AF31" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG31" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="AH31" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AI31" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AJ31" t="s" s="2">
+        <v>232</v>
+      </c>
+      <c r="AK31" t="s" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" hidden="true">
+      <c r="A32" t="s" s="2">
         <v>233</v>
-      </c>
-      <c r="AF31" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG31" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="AH31" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI31" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ31" t="s" s="2">
-        <v>141</v>
-      </c>
-      <c r="AK31" t="s" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="s" s="2">
-        <v>234</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -4481,13 +4494,13 @@
       </c>
       <c r="D32" s="2"/>
       <c r="E32" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="F32" t="s" s="2">
         <v>48</v>
       </c>
       <c r="G32" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="H32" t="s" s="2">
         <v>41</v>
@@ -4496,20 +4509,18 @@
         <v>49</v>
       </c>
       <c r="J32" t="s" s="2">
+        <v>62</v>
+      </c>
+      <c r="K32" t="s" s="2">
+        <v>234</v>
+      </c>
+      <c r="L32" t="s" s="2">
         <v>235</v>
       </c>
-      <c r="K32" t="s" s="2">
+      <c r="M32" t="s" s="2">
         <v>236</v>
       </c>
-      <c r="L32" t="s" s="2">
-        <v>237</v>
-      </c>
-      <c r="M32" t="s" s="2">
-        <v>238</v>
-      </c>
-      <c r="N32" t="s" s="2">
-        <v>239</v>
-      </c>
+      <c r="N32" s="2"/>
       <c r="O32" t="s" s="2">
         <v>41</v>
       </c>
@@ -4557,7 +4568,7 @@
         <v>41</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>39</v>
@@ -4572,19 +4583,19 @@
         <v>41</v>
       </c>
       <c r="AJ32" t="s" s="2">
-        <v>240</v>
+        <v>141</v>
       </c>
       <c r="AK32" t="s" s="2">
-        <v>241</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="2">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
-        <v>243</v>
+        <v>41</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" t="s" s="2">
@@ -4603,19 +4614,19 @@
         <v>49</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="N33" t="s" s="2">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="O33" t="s" s="2">
         <v>41</v>
@@ -4664,7 +4675,7 @@
         <v>41</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>39</v>
@@ -4679,50 +4690,50 @@
         <v>41</v>
       </c>
       <c r="AJ33" t="s" s="2">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="AK33" t="s" s="2">
-        <v>250</v>
+        <v>245</v>
       </c>
     </row>
-    <row r="34" hidden="true">
+    <row r="34">
       <c r="A34" t="s" s="2">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
-        <v>41</v>
+        <v>247</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="F34" t="s" s="2">
         <v>48</v>
       </c>
       <c r="G34" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="H34" t="s" s="2">
         <v>41</v>
       </c>
       <c r="I34" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>193</v>
+        <v>248</v>
       </c>
       <c r="K34" t="s" s="2">
+        <v>249</v>
+      </c>
+      <c r="L34" t="s" s="2">
+        <v>250</v>
+      </c>
+      <c r="M34" t="s" s="2">
+        <v>251</v>
+      </c>
+      <c r="N34" t="s" s="2">
         <v>252</v>
-      </c>
-      <c r="L34" t="s" s="2">
-        <v>253</v>
-      </c>
-      <c r="M34" t="s" s="2">
-        <v>254</v>
-      </c>
-      <c r="N34" t="s" s="2">
-        <v>255</v>
       </c>
       <c r="O34" t="s" s="2">
         <v>41</v>
@@ -4747,13 +4758,13 @@
         <v>41</v>
       </c>
       <c r="W34" t="s" s="2">
-        <v>256</v>
+        <v>41</v>
       </c>
       <c r="X34" t="s" s="2">
-        <v>257</v>
+        <v>41</v>
       </c>
       <c r="Y34" t="s" s="2">
-        <v>258</v>
+        <v>41</v>
       </c>
       <c r="Z34" t="s" s="2">
         <v>41</v>
@@ -4771,7 +4782,7 @@
         <v>41</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>39</v>
@@ -4786,15 +4797,15 @@
         <v>41</v>
       </c>
       <c r="AJ34" t="s" s="2">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="AK34" t="s" s="2">
-        <v>41</v>
+        <v>254</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -4805,10 +4816,10 @@
         <v>39</v>
       </c>
       <c r="F35" t="s" s="2">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="G35" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="H35" t="s" s="2">
         <v>41</v>
@@ -4817,16 +4828,20 @@
         <v>41</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>261</v>
+        <v>197</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>263</v>
-      </c>
-      <c r="M35" s="2"/>
-      <c r="N35" s="2"/>
+        <v>257</v>
+      </c>
+      <c r="M35" t="s" s="2">
+        <v>258</v>
+      </c>
+      <c r="N35" t="s" s="2">
+        <v>259</v>
+      </c>
       <c r="O35" t="s" s="2">
         <v>41</v>
       </c>
@@ -4850,13 +4865,13 @@
         <v>41</v>
       </c>
       <c r="W35" t="s" s="2">
-        <v>41</v>
+        <v>260</v>
       </c>
       <c r="X35" t="s" s="2">
-        <v>41</v>
+        <v>261</v>
       </c>
       <c r="Y35" t="s" s="2">
-        <v>41</v>
+        <v>262</v>
       </c>
       <c r="Z35" t="s" s="2">
         <v>41</v>
@@ -4874,13 +4889,13 @@
         <v>41</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG35" t="s" s="2">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="AH35" t="s" s="2">
         <v>41</v>
@@ -4889,7 +4904,7 @@
         <v>41</v>
       </c>
       <c r="AJ35" t="s" s="2">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="AK35" t="s" s="2">
         <v>41</v>
@@ -4897,7 +4912,7 @@
     </row>
     <row r="36">
       <c r="A36" t="s" s="2">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -4905,7 +4920,7 @@
       </c>
       <c r="D36" s="2"/>
       <c r="E36" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="F36" t="s" s="2">
         <v>40</v>
@@ -4920,17 +4935,15 @@
         <v>41</v>
       </c>
       <c r="J36" t="s" s="2">
+        <v>265</v>
+      </c>
+      <c r="K36" t="s" s="2">
         <v>266</v>
       </c>
-      <c r="K36" t="s" s="2">
+      <c r="L36" t="s" s="2">
         <v>267</v>
       </c>
-      <c r="L36" t="s" s="2">
-        <v>268</v>
-      </c>
-      <c r="M36" t="s" s="2">
-        <v>269</v>
-      </c>
+      <c r="M36" s="2"/>
       <c r="N36" s="2"/>
       <c r="O36" t="s" s="2">
         <v>41</v>
@@ -4979,7 +4992,7 @@
         <v>41</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>39</v>
@@ -4988,21 +5001,21 @@
         <v>40</v>
       </c>
       <c r="AH36" t="s" s="2">
-        <v>270</v>
+        <v>41</v>
       </c>
       <c r="AI36" t="s" s="2">
-        <v>271</v>
+        <v>41</v>
       </c>
       <c r="AJ36" t="s" s="2">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="AK36" t="s" s="2">
         <v>41</v>
       </c>
     </row>
-    <row r="37" hidden="true">
+    <row r="37">
       <c r="A37" t="s" s="2">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5010,13 +5023,13 @@
       </c>
       <c r="D37" s="2"/>
       <c r="E37" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="F37" t="s" s="2">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="G37" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="H37" t="s" s="2">
         <v>41</v>
@@ -5025,15 +5038,17 @@
         <v>41</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>62</v>
+        <v>270</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>63</v>
+        <v>271</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>64</v>
-      </c>
-      <c r="M37" s="2"/>
+        <v>272</v>
+      </c>
+      <c r="M37" t="s" s="2">
+        <v>273</v>
+      </c>
       <c r="N37" s="2"/>
       <c r="O37" t="s" s="2">
         <v>41</v>
@@ -5082,22 +5097,22 @@
         <v>41</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>65</v>
+        <v>269</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG37" t="s" s="2">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="AH37" t="s" s="2">
-        <v>41</v>
+        <v>274</v>
       </c>
       <c r="AI37" t="s" s="2">
-        <v>41</v>
+        <v>275</v>
       </c>
       <c r="AJ37" t="s" s="2">
-        <v>66</v>
+        <v>276</v>
       </c>
       <c r="AK37" t="s" s="2">
         <v>41</v>
@@ -5105,7 +5120,7 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5116,7 +5131,7 @@
         <v>39</v>
       </c>
       <c r="F38" t="s" s="2">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="G38" t="s" s="2">
         <v>41</v>
@@ -5128,13 +5143,13 @@
         <v>41</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>143</v>
+        <v>63</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>144</v>
+        <v>64</v>
       </c>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
@@ -5173,23 +5188,25 @@
         <v>41</v>
       </c>
       <c r="AA38" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AB38" s="2"/>
+        <v>41</v>
+      </c>
+      <c r="AB38" t="s" s="2">
+        <v>41</v>
+      </c>
       <c r="AC38" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AD38" t="s" s="2">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG38" t="s" s="2">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="AH38" t="s" s="2">
         <v>41</v>
@@ -5198,19 +5215,17 @@
         <v>41</v>
       </c>
       <c r="AJ38" t="s" s="2">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="AK38" t="s" s="2">
         <v>41</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>274</v>
-      </c>
-      <c r="B39" t="s" s="2">
-        <v>275</v>
-      </c>
+        <v>278</v>
+      </c>
+      <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
         <v>41</v>
       </c>
@@ -5219,10 +5234,10 @@
         <v>39</v>
       </c>
       <c r="F39" t="s" s="2">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="G39" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="H39" t="s" s="2">
         <v>41</v>
@@ -5231,13 +5246,13 @@
         <v>41</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>276</v>
+        <v>69</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>277</v>
+        <v>143</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>278</v>
+        <v>144</v>
       </c>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
@@ -5276,16 +5291,14 @@
         <v>41</v>
       </c>
       <c r="AA39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB39" t="s" s="2">
-        <v>41</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="AB39" s="2"/>
       <c r="AC39" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AD39" t="s" s="2">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="AE39" t="s" s="2">
         <v>76</v>
@@ -5297,10 +5310,10 @@
         <v>40</v>
       </c>
       <c r="AH39" t="s" s="2">
-        <v>150</v>
+        <v>41</v>
       </c>
       <c r="AI39" t="s" s="2">
-        <v>151</v>
+        <v>41</v>
       </c>
       <c r="AJ39" t="s" s="2">
         <v>41</v>
@@ -5309,42 +5322,42 @@
         <v>41</v>
       </c>
     </row>
-    <row r="40" hidden="true">
+    <row r="40">
       <c r="A40" t="s" s="2">
+        <v>278</v>
+      </c>
+      <c r="B40" t="s" s="2">
         <v>279</v>
       </c>
-      <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
-        <v>280</v>
+        <v>41</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" t="s" s="2">
         <v>39</v>
       </c>
       <c r="F40" t="s" s="2">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="G40" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="H40" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="I40" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>69</v>
+        <v>280</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>157</v>
+        <v>281</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>281</v>
-      </c>
-      <c r="M40" t="s" s="2">
-        <v>72</v>
-      </c>
+        <v>282</v>
+      </c>
+      <c r="M40" s="2"/>
       <c r="N40" s="2"/>
       <c r="O40" t="s" s="2">
         <v>41</v>
@@ -5393,7 +5406,7 @@
         <v>41</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>282</v>
+        <v>76</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>39</v>
@@ -5402,57 +5415,55 @@
         <v>40</v>
       </c>
       <c r="AH40" t="s" s="2">
-        <v>41</v>
+        <v>150</v>
       </c>
       <c r="AI40" t="s" s="2">
-        <v>41</v>
+        <v>151</v>
       </c>
       <c r="AJ40" t="s" s="2">
-        <v>141</v>
+        <v>41</v>
       </c>
       <c r="AK40" t="s" s="2">
         <v>41</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
         <v>283</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
-        <v>41</v>
+        <v>284</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" t="s" s="2">
         <v>39</v>
       </c>
       <c r="F41" t="s" s="2">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="G41" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H41" t="s" s="2">
         <v>49</v>
       </c>
-      <c r="H41" t="s" s="2">
-        <v>41</v>
-      </c>
       <c r="I41" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>193</v>
+        <v>69</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>284</v>
+        <v>161</v>
       </c>
       <c r="L41" t="s" s="2">
         <v>285</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>286</v>
-      </c>
-      <c r="N41" t="s" s="2">
-        <v>287</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="N41" s="2"/>
       <c r="O41" t="s" s="2">
         <v>41</v>
       </c>
@@ -5476,11 +5487,13 @@
         <v>41</v>
       </c>
       <c r="W41" t="s" s="2">
-        <v>171</v>
-      </c>
-      <c r="X41" s="2"/>
+        <v>41</v>
+      </c>
+      <c r="X41" t="s" s="2">
+        <v>41</v>
+      </c>
       <c r="Y41" t="s" s="2">
-        <v>288</v>
+        <v>41</v>
       </c>
       <c r="Z41" t="s" s="2">
         <v>41</v>
@@ -5498,13 +5511,13 @@
         <v>41</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG41" t="s" s="2">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="AH41" t="s" s="2">
         <v>41</v>
@@ -5513,15 +5526,15 @@
         <v>41</v>
       </c>
       <c r="AJ41" t="s" s="2">
-        <v>184</v>
+        <v>141</v>
       </c>
       <c r="AK41" t="s" s="2">
         <v>41</v>
       </c>
     </row>
-    <row r="42" hidden="true">
+    <row r="42">
       <c r="A42" t="s" s="2">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -5535,31 +5548,31 @@
         <v>48</v>
       </c>
       <c r="G42" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="H42" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="I42" t="s" s="2">
         <v>41</v>
       </c>
       <c r="J42" t="s" s="2">
+        <v>197</v>
+      </c>
+      <c r="K42" t="s" s="2">
+        <v>288</v>
+      </c>
+      <c r="L42" t="s" s="2">
+        <v>289</v>
+      </c>
+      <c r="M42" t="s" s="2">
         <v>290</v>
       </c>
-      <c r="K42" t="s" s="2">
+      <c r="N42" t="s" s="2">
         <v>291</v>
       </c>
-      <c r="L42" t="s" s="2">
-        <v>292</v>
-      </c>
-      <c r="M42" t="s" s="2">
-        <v>293</v>
-      </c>
-      <c r="N42" t="s" s="2">
-        <v>294</v>
-      </c>
       <c r="O42" t="s" s="2">
-        <v>295</v>
+        <v>41</v>
       </c>
       <c r="P42" s="2"/>
       <c r="Q42" t="s" s="2">
@@ -5581,13 +5594,11 @@
         <v>41</v>
       </c>
       <c r="W42" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="X42" t="s" s="2">
-        <v>41</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="X42" s="2"/>
       <c r="Y42" t="s" s="2">
-        <v>41</v>
+        <v>292</v>
       </c>
       <c r="Z42" t="s" s="2">
         <v>41</v>
@@ -5605,7 +5616,7 @@
         <v>41</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>39</v>
@@ -5614,13 +5625,13 @@
         <v>48</v>
       </c>
       <c r="AH42" t="s" s="2">
-        <v>296</v>
+        <v>41</v>
       </c>
       <c r="AI42" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AJ42" t="s" s="2">
-        <v>297</v>
+        <v>188</v>
       </c>
       <c r="AK42" t="s" s="2">
         <v>41</v>
@@ -5628,7 +5639,7 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -5645,28 +5656,28 @@
         <v>41</v>
       </c>
       <c r="H43" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="I43" t="s" s="2">
         <v>41</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>235</v>
+        <v>294</v>
       </c>
       <c r="K43" t="s" s="2">
+        <v>295</v>
+      </c>
+      <c r="L43" t="s" s="2">
+        <v>296</v>
+      </c>
+      <c r="M43" t="s" s="2">
+        <v>297</v>
+      </c>
+      <c r="N43" t="s" s="2">
+        <v>298</v>
+      </c>
+      <c r="O43" t="s" s="2">
         <v>299</v>
-      </c>
-      <c r="L43" t="s" s="2">
-        <v>300</v>
-      </c>
-      <c r="M43" t="s" s="2">
-        <v>301</v>
-      </c>
-      <c r="N43" t="s" s="2">
-        <v>302</v>
-      </c>
-      <c r="O43" t="s" s="2">
-        <v>41</v>
       </c>
       <c r="P43" s="2"/>
       <c r="Q43" t="s" s="2">
@@ -5712,7 +5723,7 @@
         <v>41</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>39</v>
@@ -5721,21 +5732,21 @@
         <v>48</v>
       </c>
       <c r="AH43" t="s" s="2">
-        <v>41</v>
+        <v>300</v>
       </c>
       <c r="AI43" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AJ43" t="s" s="2">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="AK43" t="s" s="2">
         <v>41</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -5743,13 +5754,13 @@
       </c>
       <c r="D44" s="2"/>
       <c r="E44" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="F44" t="s" s="2">
         <v>48</v>
       </c>
       <c r="G44" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="H44" t="s" s="2">
         <v>41</v>
@@ -5758,16 +5769,20 @@
         <v>41</v>
       </c>
       <c r="J44" t="s" s="2">
+        <v>239</v>
+      </c>
+      <c r="K44" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="L44" t="s" s="2">
+        <v>304</v>
+      </c>
+      <c r="M44" t="s" s="2">
         <v>305</v>
       </c>
-      <c r="K44" t="s" s="2">
+      <c r="N44" t="s" s="2">
         <v>306</v>
       </c>
-      <c r="L44" t="s" s="2">
-        <v>307</v>
-      </c>
-      <c r="M44" s="2"/>
-      <c r="N44" s="2"/>
       <c r="O44" t="s" s="2">
         <v>41</v>
       </c>
@@ -5815,10 +5830,10 @@
         <v>41</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>48</v>
@@ -5830,15 +5845,15 @@
         <v>41</v>
       </c>
       <c r="AJ44" t="s" s="2">
+        <v>307</v>
+      </c>
+      <c r="AK44" t="s" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="2">
         <v>308</v>
-      </c>
-      <c r="AK44" t="s" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="45" hidden="true">
-      <c r="A45" t="s" s="2">
-        <v>309</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -5846,13 +5861,13 @@
       </c>
       <c r="D45" s="2"/>
       <c r="E45" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="F45" t="s" s="2">
         <v>48</v>
       </c>
       <c r="G45" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="H45" t="s" s="2">
         <v>41</v>
@@ -5861,13 +5876,13 @@
         <v>41</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>62</v>
+        <v>309</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>63</v>
+        <v>310</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>64</v>
+        <v>311</v>
       </c>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
@@ -5918,10 +5933,10 @@
         <v>41</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>65</v>
+        <v>308</v>
       </c>
       <c r="AF45" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="AG45" t="s" s="2">
         <v>48</v>
@@ -5933,7 +5948,7 @@
         <v>41</v>
       </c>
       <c r="AJ45" t="s" s="2">
-        <v>66</v>
+        <v>312</v>
       </c>
       <c r="AK45" t="s" s="2">
         <v>41</v>
@@ -5941,18 +5956,18 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
-        <v>68</v>
+        <v>41</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" t="s" s="2">
         <v>39</v>
       </c>
       <c r="F46" t="s" s="2">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="G46" t="s" s="2">
         <v>41</v>
@@ -5964,17 +5979,15 @@
         <v>41</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="M46" t="s" s="2">
-        <v>72</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="M46" s="2"/>
       <c r="N46" s="2"/>
       <c r="O46" t="s" s="2">
         <v>41</v>
@@ -6011,25 +6024,25 @@
         <v>41</v>
       </c>
       <c r="AA46" t="s" s="2">
-        <v>73</v>
+        <v>41</v>
       </c>
       <c r="AB46" t="s" s="2">
-        <v>74</v>
+        <v>41</v>
       </c>
       <c r="AC46" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AD46" t="s" s="2">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG46" t="s" s="2">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="AH46" t="s" s="2">
         <v>41</v>
@@ -6046,18 +6059,18 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
-        <v>41</v>
+        <v>68</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="F47" t="s" s="2">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="G47" t="s" s="2">
         <v>41</v>
@@ -6066,19 +6079,19 @@
         <v>41</v>
       </c>
       <c r="I47" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>218</v>
+        <v>70</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>219</v>
+        <v>71</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>220</v>
+        <v>72</v>
       </c>
       <c r="N47" s="2"/>
       <c r="O47" t="s" s="2">
@@ -6116,34 +6129,34 @@
         <v>41</v>
       </c>
       <c r="AA47" t="s" s="2">
-        <v>41</v>
+        <v>73</v>
       </c>
       <c r="AB47" t="s" s="2">
-        <v>41</v>
+        <v>74</v>
       </c>
       <c r="AC47" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AD47" t="s" s="2">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>221</v>
+        <v>76</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG47" t="s" s="2">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="AH47" t="s" s="2">
-        <v>222</v>
+        <v>41</v>
       </c>
       <c r="AI47" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AJ47" t="s" s="2">
-        <v>141</v>
+        <v>66</v>
       </c>
       <c r="AK47" t="s" s="2">
         <v>41</v>
@@ -6151,7 +6164,7 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -6159,7 +6172,7 @@
       </c>
       <c r="D48" s="2"/>
       <c r="E48" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="F48" t="s" s="2">
         <v>48</v>
@@ -6174,16 +6187,16 @@
         <v>49</v>
       </c>
       <c r="J48" t="s" s="2">
-        <v>161</v>
+        <v>62</v>
       </c>
       <c r="K48" t="s" s="2">
+        <v>222</v>
+      </c>
+      <c r="L48" t="s" s="2">
+        <v>223</v>
+      </c>
+      <c r="M48" t="s" s="2">
         <v>224</v>
-      </c>
-      <c r="L48" t="s" s="2">
-        <v>225</v>
-      </c>
-      <c r="M48" t="s" s="2">
-        <v>226</v>
       </c>
       <c r="N48" s="2"/>
       <c r="O48" t="s" s="2">
@@ -6233,7 +6246,7 @@
         <v>41</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>39</v>
@@ -6242,13 +6255,13 @@
         <v>48</v>
       </c>
       <c r="AH48" t="s" s="2">
-        <v>41</v>
+        <v>226</v>
       </c>
       <c r="AI48" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AJ48" t="s" s="2">
-        <v>228</v>
+        <v>141</v>
       </c>
       <c r="AK48" t="s" s="2">
         <v>41</v>
@@ -6256,7 +6269,7 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -6279,16 +6292,16 @@
         <v>49</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>62</v>
+        <v>165</v>
       </c>
       <c r="K49" t="s" s="2">
+        <v>228</v>
+      </c>
+      <c r="L49" t="s" s="2">
+        <v>229</v>
+      </c>
+      <c r="M49" t="s" s="2">
         <v>230</v>
-      </c>
-      <c r="L49" t="s" s="2">
-        <v>231</v>
-      </c>
-      <c r="M49" t="s" s="2">
-        <v>232</v>
       </c>
       <c r="N49" s="2"/>
       <c r="O49" t="s" s="2">
@@ -6338,7 +6351,7 @@
         <v>41</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>39</v>
@@ -6353,7 +6366,7 @@
         <v>41</v>
       </c>
       <c r="AJ49" t="s" s="2">
-        <v>141</v>
+        <v>232</v>
       </c>
       <c r="AK49" t="s" s="2">
         <v>41</v>
@@ -6361,7 +6374,7 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -6381,23 +6394,21 @@
         <v>41</v>
       </c>
       <c r="I50" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="J50" t="s" s="2">
-        <v>193</v>
+        <v>62</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>315</v>
+        <v>234</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>316</v>
+        <v>235</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>317</v>
-      </c>
-      <c r="N50" t="s" s="2">
-        <v>318</v>
-      </c>
+        <v>236</v>
+      </c>
+      <c r="N50" s="2"/>
       <c r="O50" t="s" s="2">
         <v>41</v>
       </c>
@@ -6421,53 +6432,160 @@
         <v>41</v>
       </c>
       <c r="W50" t="s" s="2">
-        <v>256</v>
+        <v>41</v>
       </c>
       <c r="X50" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Y50" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Z50" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA50" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AB50" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AC50" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD50" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AE50" t="s" s="2">
+        <v>237</v>
+      </c>
+      <c r="AF50" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG50" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="AH50" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AI50" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AJ50" t="s" s="2">
+        <v>141</v>
+      </c>
+      <c r="AK50" t="s" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="51" hidden="true">
+      <c r="A51" t="s" s="2">
+        <v>318</v>
+      </c>
+      <c r="B51" s="2"/>
+      <c r="C51" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="D51" s="2"/>
+      <c r="E51" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="F51" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="G51" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H51" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="I51" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="J51" t="s" s="2">
+        <v>197</v>
+      </c>
+      <c r="K51" t="s" s="2">
         <v>319</v>
       </c>
-      <c r="Y50" t="s" s="2">
+      <c r="L51" t="s" s="2">
         <v>320</v>
       </c>
-      <c r="Z50" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA50" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB50" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC50" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD50" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE50" t="s" s="2">
-        <v>314</v>
-      </c>
-      <c r="AF50" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG50" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="AH50" t="s" s="2">
-        <v>270</v>
-      </c>
-      <c r="AI50" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ50" t="s" s="2">
+      <c r="M51" t="s" s="2">
         <v>321</v>
       </c>
-      <c r="AK50" t="s" s="2">
+      <c r="N51" t="s" s="2">
+        <v>322</v>
+      </c>
+      <c r="O51" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="P51" s="2"/>
+      <c r="Q51" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="R51" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="S51" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="T51" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="U51" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="V51" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="W51" t="s" s="2">
+        <v>260</v>
+      </c>
+      <c r="X51" t="s" s="2">
+        <v>323</v>
+      </c>
+      <c r="Y51" t="s" s="2">
+        <v>324</v>
+      </c>
+      <c r="Z51" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA51" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AB51" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AC51" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD51" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AE51" t="s" s="2">
+        <v>318</v>
+      </c>
+      <c r="AF51" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG51" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="AH51" t="s" s="2">
+        <v>274</v>
+      </c>
+      <c r="AI51" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AJ51" t="s" s="2">
+        <v>325</v>
+      </c>
+      <c r="AK51" t="s" s="2">
         <v>41</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AK50">
+  <autoFilter ref="A1:AK51">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -6477,7 +6595,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI49">
+  <conditionalFormatting sqref="A2:AI50">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>